<commit_message>
Add idle anim for bat
</commit_message>
<xml_diff>
--- a/ExcelData/final-roguelike-design.xlsx
+++ b/ExcelData/final-roguelike-design.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\final-roguelike\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539D714C-17AE-4CDE-868A-A2059F386275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49254C4F-520F-4838-96DB-5F1AD346CD17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="510" yWindow="3165" windowWidth="19140" windowHeight="11880" activeTab="2" xr2:uid="{6E43F2A3-315C-41BF-846A-15AE66A53DEC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{6E43F2A3-315C-41BF-846A-15AE66A53DEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Constant" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="128">
   <si>
     <t>MAX_ATK_SPD</t>
   </si>
@@ -467,6 +467,18 @@
   <si>
     <t>+ 20% coin drops from enemy
 + 10% coin drops from chest</t>
+  </si>
+  <si>
+    <t>Armor</t>
+  </si>
+  <si>
+    <t>Leather Armor</t>
+  </si>
+  <si>
+    <t>+ 10 Damage</t>
+  </si>
+  <si>
+    <t>Steal Armor</t>
   </si>
 </sst>
 </file>
@@ -1318,11 +1330,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01335834-5C35-42F1-8C7C-B06238121802}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,7 +1363,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>24</v>
       </c>
@@ -1369,7 +1381,7 @@
       </c>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>24</v>
       </c>
@@ -1387,7 +1399,7 @@
       </c>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>24</v>
       </c>
@@ -1405,7 +1417,7 @@
       </c>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>24</v>
       </c>
@@ -1423,7 +1435,7 @@
       </c>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>24</v>
       </c>
@@ -1441,7 +1453,7 @@
       </c>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>24</v>
       </c>
@@ -1459,7 +1471,7 @@
       </c>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>24</v>
       </c>
@@ -1477,7 +1489,7 @@
       </c>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>24</v>
       </c>
@@ -1495,7 +1507,7 @@
       </c>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>24</v>
       </c>
@@ -1512,7 +1524,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>24</v>
       </c>
@@ -1530,7 +1542,7 @@
       </c>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>24</v>
       </c>
@@ -1548,7 +1560,7 @@
       </c>
       <c r="F12" s="9"/>
     </row>
-    <row r="13" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>24</v>
       </c>
@@ -1566,7 +1578,7 @@
       </c>
       <c r="F13" s="9"/>
     </row>
-    <row r="14" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>24</v>
       </c>
@@ -1598,7 +1610,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>24</v>
       </c>
@@ -1630,7 +1642,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>24</v>
       </c>
@@ -1662,7 +1674,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>24</v>
       </c>
@@ -1679,7 +1691,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>24</v>
       </c>
@@ -1696,7 +1708,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>24</v>
       </c>
@@ -1713,7 +1725,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>24</v>
       </c>
@@ -1731,78 +1743,220 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D24" s="11"/>
+      <c r="A24" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D25" s="11"/>
+      <c r="A25" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="D26" s="11"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="D27" s="11"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="D28" s="11"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="D29" s="11"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="D30" s="11"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="D31" s="11"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="D32" s="11"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="D33" s="11"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="D34" s="11"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="D35" s="11"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="D36" s="11"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="D37" s="11"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="D38" s="11"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="D39" s="11"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="D40" s="11"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="D41" s="11"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="D42" s="11"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>114</v>
+      </c>
       <c r="D43" s="11"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>114</v>
+      </c>
       <c r="D44" s="11"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="D45" s="11"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D46" s="11"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D47" s="11"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D48" s="11"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2204,11 +2358,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E79" xr:uid="{01335834-5C35-42F1-8C7C-B06238121802}">
-    <filterColumn colId="4">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:E79" xr:uid="{01335834-5C35-42F1-8C7C-B06238121802}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>